<commit_message>
New modelling cycle python code
This new code takes the new variable safety time into account. This new safety time is based on the passenger count of the plane. This passenger count is randomly assigned is a predetermined interval. This new code also works for the original non variable safety time.

Co-Authored-By: Shae Williams <17145933+Shaetje1@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data_small_extended.xlsx
+++ b/data_small_extended.xlsx
@@ -8,21 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FvTop\Documents\GitHub\airplane-math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1524D2A9-7D61-4310-8C8B-6078DA19062F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98206ECF-BEA3-48ED-8658-92DAE94CF9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2760" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General information" sheetId="1" r:id="rId1"/>
     <sheet name="Times per aircraft" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Number of aircrafts</t>
   </si>
@@ -58,6 +70,9 @@
   </si>
   <si>
     <t>Added safety time</t>
+  </si>
+  <si>
+    <t>New safety time:</t>
   </si>
 </sst>
 </file>
@@ -447,7 +462,7 @@
   <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,10 +731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,9 +744,11 @@
     <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -750,8 +767,11 @@
       <c r="F1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -770,8 +790,12 @@
       <c r="F2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <f>'General information'!$B$2+'Times per aircraft'!F2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -790,8 +814,12 @@
       <c r="F3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>'General information'!$B$2+'Times per aircraft'!F3</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -810,8 +838,12 @@
       <c r="F4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f>'General information'!$B$2+'Times per aircraft'!F4</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -830,8 +862,12 @@
       <c r="F5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <f>'General information'!$B$2+'Times per aircraft'!F5</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -850,8 +886,12 @@
       <c r="F6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <f>'General information'!$B$2+'Times per aircraft'!F6</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -870,8 +910,12 @@
       <c r="F7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <f>'General information'!$B$2+'Times per aircraft'!F7</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -890,8 +934,12 @@
       <c r="F8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f>'General information'!$B$2+'Times per aircraft'!F8</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -910,8 +958,12 @@
       <c r="F9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f>'General information'!$B$2+'Times per aircraft'!F9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -930,8 +982,12 @@
       <c r="F10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>'General information'!$B$2+'Times per aircraft'!F10</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -950,17 +1006,21 @@
       <c r="F11">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f>'General information'!$B$2+'Times per aircraft'!F11</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>